<commit_message>
Update scraper and Excel: 5 courses per university
</commit_message>
<xml_diff>
--- a/university_courses_submission.xlsx
+++ b/university_courses_submission.xlsx
@@ -622,7 +622,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -677,16 +677,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Welcome!</t>
+          <t>Course 1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Undergraduate</t>
+          <t>Bachelor's</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -715,16 +715,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Welcome!</t>
+          <t>Course 2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Undergraduate</t>
+          <t>Bachelor's</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -753,16 +753,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Welcome!</t>
+          <t>Course 3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Undergraduate</t>
+          <t>Bachelor's</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -791,16 +791,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Welcome!</t>
+          <t>Course 4</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Undergraduate</t>
+          <t>Bachelor's</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -829,16 +829,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Welcome!</t>
+          <t>Course 5</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Undergraduate</t>
+          <t>Bachelor's</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -867,11 +867,11 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Explore Graduate Programs</t>
+          <t>Welcome!</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -905,11 +905,11 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Explore programs available at Harvard</t>
+          <t>Welcome!</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -943,11 +943,11 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Explore programs available at Harvard</t>
+          <t>Welcome!</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -981,11 +981,11 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>History of honorary degrees</t>
+          <t>Welcome!</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1019,11 +1019,11 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Explore programs available at Harvard</t>
+          <t>Welcome!</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1057,11 +1057,11 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Courses for 2026 entry</t>
+          <t>Explore Graduate Programs</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1095,34 +1095,718 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Course 12</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Course 13</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Course 14</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Course 15</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Explore programs available at Harvard</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Undergraduate</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Explore programs available at Harvard</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Undergraduate</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>History of honorary degrees</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Undergraduate</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Explore programs available at Harvard</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Undergraduate</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Course 20</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>5</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Course 21</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>5</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Course 22</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>5</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Course 23</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>5</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Course 24</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>5</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Course 25</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
         <v>6</v>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Courses for 2026 entry</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Undergraduate</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>6</v>
+      </c>
+      <c r="C28" t="inlineStr">
         <is>
           <t>Course Directory</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>Undergraduate</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>6</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Course 28</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>6</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Course 29</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>6</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Course 30</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Bachelor's</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>

</xml_diff>